<commit_message>
moved uav to correct id
</commit_message>
<xml_diff>
--- a/xBee_to_Platform.xlsx
+++ b/xBee_to_Platform.xlsx
@@ -487,7 +487,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +537,9 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
       <c r="D4">
         <v>2</v>
       </c>
@@ -549,7 +552,7 @@
         <v>7974</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -561,9 +564,6 @@
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
       </c>
       <c r="D6">
         <v>4</v>

</xml_diff>